<commit_message>
round robin (not balanced) results
</commit_message>
<xml_diff>
--- a/training_results_by_epoch_round_robin.xlsx
+++ b/training_results_by_epoch_round_robin.xlsx
@@ -488,28 +488,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6365870786516854</v>
+        <v>0.6402153558052435</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6307580319156455</v>
+        <v>0.6305742837354592</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3584628401089932</v>
+        <v>0.2764798242788156</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5419359835587747</v>
+        <v>0.5157564879398394</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5049954586739328</v>
+        <v>0.5004541326067211</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6251236888976845</v>
+        <v>0.624727884425094</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3056445309657391</v>
+        <v>0.2453740332067915</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4785878928457855</v>
+        <v>0.4568520167462022</v>
       </c>
     </row>
     <row r="3">
@@ -520,28 +520,28 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.75187265917603</v>
+        <v>0.7652153558052435</v>
       </c>
       <c r="D3" t="n">
-        <v>0.632948875602482</v>
+        <v>0.7285968706271466</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4512066287119473</v>
+        <v>0.3782158706398598</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6120093878301531</v>
+        <v>0.6240093656907499</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4977293369663942</v>
+        <v>0.485921889191644</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6277953690876706</v>
+        <v>0.722343162477736</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3253789523850333</v>
+        <v>0.3270598505952984</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4836345528130327</v>
+        <v>0.5117749674215595</v>
       </c>
     </row>
     <row r="4">
@@ -552,28 +552,28 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8561563670411985</v>
+        <v>0.8886938202247191</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6376415214349319</v>
+        <v>0.7496289700207777</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5629619662352371</v>
+        <v>0.4736095964292549</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6855866182371225</v>
+        <v>0.7039774622249172</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5022706630336058</v>
+        <v>0.5140781108083561</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6330892539085692</v>
+        <v>0.7346625766871165</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3676530789168332</v>
+        <v>0.3972993705211142</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5010043319530028</v>
+        <v>0.5486800193388622</v>
       </c>
     </row>
     <row r="5">
@@ -584,28 +584,28 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9205290262172284</v>
+        <v>0.9046114232209738</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6431539668405207</v>
+        <v>0.7607457349220483</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6257291563806273</v>
+        <v>0.4996195511294804</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7298040498127921</v>
+        <v>0.7216589030908341</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5040871934604905</v>
+        <v>0.5059037238873751</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6402137344151989</v>
+        <v>0.7424797150207797</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3714821446850872</v>
+        <v>0.3815912287648544</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5052610241869256</v>
+        <v>0.5433248892243364</v>
       </c>
     </row>
     <row r="6">
@@ -616,28 +616,28 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9763576779026217</v>
+        <v>0.9702715355805244</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6748999985865525</v>
+        <v>0.7621097117980467</v>
       </c>
       <c r="E6" t="n">
-        <v>0.677871873245405</v>
+        <v>0.5650893777043705</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7763765165781931</v>
+        <v>0.7658235416943139</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5040871934604905</v>
+        <v>0.5059037238873751</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6704927765683752</v>
+        <v>0.7403522659806056</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3496550841280678</v>
+        <v>0.3962485499877949</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5080783513856445</v>
+        <v>0.5475015132852584</v>
       </c>
     </row>
     <row r="7">
@@ -648,28 +648,28 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9715589887640449</v>
+        <v>0.9731975655430711</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6867234872577704</v>
+        <v>0.7770710540078305</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7368908406832592</v>
+        <v>0.6177959043413878</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7983911055683581</v>
+        <v>0.7893548412974298</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5231607629427792</v>
+        <v>0.5095367847411444</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6848406886997823</v>
+        <v>0.7522758757173956</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3830343672751008</v>
+        <v>0.4126899351101684</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5303452729725541</v>
+        <v>0.5581675318562361</v>
       </c>
     </row>
     <row r="8">
@@ -680,28 +680,28 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.983497191011236</v>
+        <v>0.9860720973782772</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7153599344160342</v>
+        <v>0.7789368047604913</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7740662743727545</v>
+        <v>0.6670591584846525</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8243077999333416</v>
+        <v>0.8106893535411404</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5077202543142597</v>
+        <v>0.5122615803814714</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7130417573718583</v>
+        <v>0.7485652087868593</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3532272888912163</v>
+        <v>0.4198586675077124</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5246631001924448</v>
+        <v>0.5602284855586811</v>
       </c>
     </row>
     <row r="9">
@@ -712,28 +712,28 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9856039325842697</v>
+        <v>0.9832631086142322</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7274166419313347</v>
+        <v>0.7890288201953385</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8085426696089318</v>
+        <v>0.7072696882658795</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8405210813748454</v>
+        <v>0.8265205390251501</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4913714804722979</v>
+        <v>0.5095367847411444</v>
       </c>
       <c r="H9" t="n">
-        <v>0.7254106471403127</v>
+        <v>0.7558875915297842</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3952668787958332</v>
+        <v>0.4328464779303688</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5373496688028145</v>
+        <v>0.5660902847337658</v>
       </c>
     </row>
     <row r="10">
@@ -744,28 +744,28 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9885299625468165</v>
+        <v>0.9928604868913857</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7369786145387214</v>
+        <v>0.7932055576757269</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8316232500996982</v>
+        <v>0.7556263227652499</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8523772757284119</v>
+        <v>0.8472307891107875</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5068119891008175</v>
+        <v>0.5204359673024523</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7309024341975064</v>
+        <v>0.7571739560657036</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4002531118110201</v>
+        <v>0.4568105041770552</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5459891783697813</v>
+        <v>0.5781401425150704</v>
       </c>
     </row>
     <row r="11">
@@ -776,28 +776,28 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9893492509363296</v>
+        <v>0.9952013108614233</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7391977271763559</v>
+        <v>0.8005201486946812</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8472039950036634</v>
+        <v>0.7836565374349646</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8585836577054496</v>
+        <v>0.8597926656636897</v>
       </c>
       <c r="G11" t="n">
-        <v>0.516802906448683</v>
+        <v>0.5277020890099909</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7318919453789828</v>
+        <v>0.759499307342173</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3845377445910495</v>
+        <v>0.4565078155115433</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5444108654729051</v>
+        <v>0.5812364039545691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>